<commit_message>
Correction categories dataschema longitudinal
</commit_message>
<xml_diff>
--- a/longitudinal/dataschema_ProPASS_longitudinal.xlsx
+++ b/longitudinal/dataschema_ProPASS_longitudinal.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/849507f40a0f895e/Documents/ProPASS/DataSchema/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindsey\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{788F9B1B-ACAA-424E-AB36-167FC8EEAB69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A57A83-01E7-4581-808B-02234F5270F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="465" windowWidth="29040" windowHeight="15720" xr2:uid="{FC4A5C44-0DEC-4188-833A-37731883B462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FC4A5C44-0DEC-4188-833A-37731883B462}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="345">
   <si>
     <t>index</t>
   </si>
@@ -120,9 +120,6 @@
     <t>questionnaire</t>
   </si>
   <si>
-    <t>sdc_f1_sex</t>
-  </si>
-  <si>
     <t>Sex</t>
   </si>
   <si>
@@ -138,18 +135,12 @@
     <t>years</t>
   </si>
   <si>
-    <t>sdc_f1_education</t>
-  </si>
-  <si>
     <t>Level of education</t>
   </si>
   <si>
     <t>Participant's level of education at the time of questionnaire completion</t>
   </si>
   <si>
-    <t>sdc_f1_employment_status</t>
-  </si>
-  <si>
     <t>Current employment status</t>
   </si>
   <si>
@@ -159,9 +150,6 @@
     <t>Homemaker/housewife/househusband considered as unemployed. Rentier considered as employed. Students, apprentices, retired, and family workers considered as NA.</t>
   </si>
   <si>
-    <t>sdc_f1_employment_pattern</t>
-  </si>
-  <si>
     <t>Current employment pattern</t>
   </si>
   <si>
@@ -186,9 +174,6 @@
     <t>Participant's employment description</t>
   </si>
   <si>
-    <t>sdc_f1_retirement_status</t>
-  </si>
-  <si>
     <t>Current retirement status</t>
   </si>
   <si>
@@ -198,27 +183,18 @@
     <t>Students and voluntary workers set as NA. Accept categories that combine retired and pensioner.</t>
   </si>
   <si>
-    <t>sdc_f1_married</t>
-  </si>
-  <si>
     <t>Ever married</t>
   </si>
   <si>
     <t>Indicator of whether the participant has ever been married or not</t>
   </si>
   <si>
-    <t>sdc_f1_relationship</t>
-  </si>
-  <si>
     <t>Currently in a formal relationship</t>
   </si>
   <si>
     <t>Indicator of whether the participant is in a formal relationship or not</t>
   </si>
   <si>
-    <t>sdc_f1_location</t>
-  </si>
-  <si>
     <t>Urban or rural location</t>
   </si>
   <si>
@@ -228,9 +204,6 @@
     <t>cm</t>
   </si>
   <si>
-    <t>pm_f1_height_method</t>
-  </si>
-  <si>
     <t>Method used to measure the height</t>
   </si>
   <si>
@@ -240,9 +213,6 @@
     <t>kg</t>
   </si>
   <si>
-    <t>pm_f1_weight_method</t>
-  </si>
-  <si>
     <t>Method used to measure the weight</t>
   </si>
   <si>
@@ -258,9 +228,6 @@
     <t>Waist circumference</t>
   </si>
   <si>
-    <t>pm_f1_waist_circ_method</t>
-  </si>
-  <si>
     <t>Method used to measure the waist circumference</t>
   </si>
   <si>
@@ -306,9 +273,6 @@
     <t>Method can differ but must be detailed in harmonization comment</t>
   </si>
   <si>
-    <t>lab_f1_blood_fasting</t>
-  </si>
-  <si>
     <t>Blood sampling fasting</t>
   </si>
   <si>
@@ -357,9 +321,6 @@
     <t>g/day</t>
   </si>
   <si>
-    <t>nut_f1_fruit_frequency</t>
-  </si>
-  <si>
     <t>Fruit intake frequency</t>
   </si>
   <si>
@@ -372,9 +333,6 @@
     <t>Vegetable Intake quantity</t>
   </si>
   <si>
-    <t>nut_f1_vegetable_frequency</t>
-  </si>
-  <si>
     <t>Vegetable intake frequency</t>
   </si>
   <si>
@@ -396,15 +354,9 @@
     <t>g/week</t>
   </si>
   <si>
-    <t>alc_f1_alcohol_frequency</t>
-  </si>
-  <si>
     <t>Frequency of alcohol consumption</t>
   </si>
   <si>
-    <t>smk_f1_smoking_status</t>
-  </si>
-  <si>
     <t>Smoking status</t>
   </si>
   <si>
@@ -414,9 +366,6 @@
     <t>Occasional smokers considered as smokers.</t>
   </si>
   <si>
-    <t>smk_f1_smoking_frequency</t>
-  </si>
-  <si>
     <t>Current smoking frequency</t>
   </si>
   <si>
@@ -426,15 +375,9 @@
     <t>cigarettes/week</t>
   </si>
   <si>
-    <t>lsb_f1_rated_health</t>
-  </si>
-  <si>
     <t>Self Rated Health</t>
   </si>
   <si>
-    <t>dis_f1_cvd</t>
-  </si>
-  <si>
     <t>Cardio vascular diseases</t>
   </si>
   <si>
@@ -444,66 +387,39 @@
     <t>When studies don't have a "other" category the "No" cannot be generated. In this situation only 1 and NA would be present.</t>
   </si>
   <si>
-    <t>dis_f1_musculoskeletal</t>
-  </si>
-  <si>
     <t>Musculoskeletal diseases</t>
   </si>
   <si>
     <t>Musculoskeletal diseases (osteoporosis, arthrosis, rheumatic disorder, osteoarthritis or rheumatism, rheumatoid arthritis, osteoarthritis, other arthritis, rheumatoid arthritis)</t>
   </si>
   <si>
-    <t>dis_f1_diabetes</t>
-  </si>
-  <si>
     <t>Diabetes</t>
   </si>
   <si>
     <t>Diabetes (including gestational diabetes and other types of diabetes but excluding impaired fasting glucose and impaired glucose tolerance)</t>
   </si>
   <si>
-    <t>dis_f1_diabetes_type</t>
-  </si>
-  <si>
     <t>Diabetes type</t>
   </si>
   <si>
     <t>Diabetes type (including gestational diabetes and other types of diabetes but excluding impaired fasting glucose and impaired glucose tolerance)</t>
   </si>
   <si>
-    <t>dis_f1_cancer</t>
-  </si>
-  <si>
     <t>Cancer</t>
   </si>
   <si>
-    <t>dis_f1_hypercholesteromia</t>
-  </si>
-  <si>
     <t>Diagnosed hypercholesteromia</t>
   </si>
   <si>
-    <t>med_f1_lipid_lowering</t>
-  </si>
-  <si>
     <t>Current use of lipid lowering medication</t>
   </si>
   <si>
-    <t>med_f1_blood_pressure</t>
-  </si>
-  <si>
     <t>Current use of medication to manage blood pressure</t>
   </si>
   <si>
-    <t>med_f1_diabetes</t>
-  </si>
-  <si>
     <t>Current use of medication for diabetes</t>
   </si>
   <si>
-    <t>cog_f1_depression</t>
-  </si>
-  <si>
     <t>Depression</t>
   </si>
   <si>
@@ -531,9 +447,6 @@
     <t>MoCa score</t>
   </si>
   <si>
-    <t>cog_f1_alzheimers_dementia</t>
-  </si>
-  <si>
     <t>Alzheimers/Dementia</t>
   </si>
   <si>
@@ -543,60 +456,36 @@
     <t>hours</t>
   </si>
   <si>
-    <t>sleep_f1_duration_cat</t>
-  </si>
-  <si>
     <t>Usual number of hours of sleep - categorical</t>
   </si>
   <si>
-    <t>sleep_f1_difficulties</t>
-  </si>
-  <si>
     <t>Indicator of whether the participant has difficulties sleeping or not</t>
   </si>
   <si>
-    <t>sed_f1_beh_tv_week_all</t>
-  </si>
-  <si>
     <t>Daily TV viewing during the week</t>
   </si>
   <si>
     <t>Calculate weighted average if needed</t>
   </si>
   <si>
-    <t>sed_f1_beh_tv_week_days</t>
-  </si>
-  <si>
     <t>Daily TV viewing during week days</t>
   </si>
   <si>
-    <t>sed_f1_beh_tv_weekend_days</t>
-  </si>
-  <si>
     <t>Daily TV viewing during weekend days</t>
   </si>
   <si>
-    <t>sed_f1_beh_comp_use</t>
-  </si>
-  <si>
     <t>Computer use</t>
   </si>
   <si>
     <t>Time spent using a computer per day on weekdays excluding computer use at work</t>
   </si>
   <si>
-    <t>sed_f1_beh_video_games</t>
-  </si>
-  <si>
     <t>Video games</t>
   </si>
   <si>
     <t>Time spent playing video games per day</t>
   </si>
   <si>
-    <t>sed_f1_beh_reading</t>
-  </si>
-  <si>
     <t>Reading</t>
   </si>
   <si>
@@ -609,33 +498,21 @@
     <t>Overall time spent sitting per day</t>
   </si>
   <si>
-    <t>sed_f1_beh_total_sitting_cat</t>
-  </si>
-  <si>
     <t>Total sitting time per day - categorical</t>
   </si>
   <si>
     <t>Overall time spent sitting per day - categorical</t>
   </si>
   <si>
-    <t>phy_f1_walking</t>
-  </si>
-  <si>
     <t>Walking for leisure</t>
   </si>
   <si>
     <t>Frequency of walking for leisure per week</t>
   </si>
   <si>
-    <t>phy_f1_occupational_pa</t>
-  </si>
-  <si>
     <t>Occupational physical activity</t>
   </si>
   <si>
-    <t>phy_f1_sport_participation</t>
-  </si>
-  <si>
     <t>Sport participation</t>
   </si>
   <si>
@@ -645,18 +522,12 @@
     <t>When studies don't have a "other" category the "No" cannot be generated. In this situation only 1 and NA would be present. Physical activity was considered as sport as soon as the intensity was specified as being moderate or more.</t>
   </si>
   <si>
-    <t>phy_f1_active_commuting</t>
-  </si>
-  <si>
     <t>Active commuting</t>
   </si>
   <si>
     <t>Indicator of whether the participant is engaging in active commuting</t>
   </si>
   <si>
-    <t>phy_f1_leisure_time</t>
-  </si>
-  <si>
     <t>Leisure-time physical activity, including sport</t>
   </si>
   <si>
@@ -681,9 +552,6 @@
     <t>items</t>
   </si>
   <si>
-    <t>death_f1_status</t>
-  </si>
-  <si>
     <t>project</t>
   </si>
   <si>
@@ -1201,6 +1069,9 @@
   </si>
   <si>
     <t>phy_SF36_nb_items</t>
+  </si>
+  <si>
+    <t>death_status</t>
   </si>
 </sst>
 </file>
@@ -1574,8 +1445,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138A0E81-F778-497B-A6EC-B26BAFD348B9}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1683,7 +1554,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>307</v>
+        <v>263</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1712,13 +1583,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>308</v>
+        <v>264</v>
       </c>
       <c r="D5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" t="s">
         <v>28</v>
-      </c>
-      <c r="E5" t="s">
-        <v>29</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -1738,19 +1609,19 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>309</v>
+        <v>265</v>
       </c>
       <c r="D6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" t="s">
         <v>30</v>
-      </c>
-      <c r="E6" t="s">
-        <v>31</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
         <v>25</v>
@@ -1767,13 +1638,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>310</v>
+        <v>266</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E7" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
@@ -1793,13 +1664,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>311</v>
+        <v>267</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="E8" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
@@ -1811,7 +1682,7 @@
         <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
@@ -1822,13 +1693,13 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>312</v>
+        <v>268</v>
       </c>
       <c r="D9" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="E9" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
@@ -1840,7 +1711,7 @@
         <v>26</v>
       </c>
       <c r="L9" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -1851,16 +1722,16 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>313</v>
+        <v>269</v>
       </c>
       <c r="D10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="E10" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="F10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I10" t="s">
         <v>25</v>
@@ -1877,13 +1748,13 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>314</v>
+        <v>270</v>
       </c>
       <c r="D11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
         <v>16</v>
@@ -1903,13 +1774,13 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>315</v>
+        <v>271</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
@@ -1921,7 +1792,7 @@
         <v>26</v>
       </c>
       <c r="L12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -1932,13 +1803,13 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>316</v>
+        <v>272</v>
       </c>
       <c r="D13" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="E13" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
@@ -1958,13 +1829,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>317</v>
+        <v>273</v>
       </c>
       <c r="D14" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="E14" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
@@ -1984,13 +1855,13 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>318</v>
+        <v>274</v>
       </c>
       <c r="D15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E15" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
@@ -2010,19 +1881,19 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>319</v>
+        <v>275</v>
       </c>
       <c r="D16" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="E16" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="F16" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G16" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I16" t="s">
         <v>25</v>
@@ -2039,13 +1910,13 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>320</v>
+        <v>276</v>
       </c>
       <c r="D17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="E17" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
@@ -2065,19 +1936,19 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>321</v>
+        <v>277</v>
       </c>
       <c r="D18" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="E18" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="F18" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G18" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I18" t="s">
         <v>25</v>
@@ -2094,13 +1965,13 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>322</v>
+        <v>278</v>
       </c>
       <c r="D19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="E19" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
@@ -2120,19 +1991,19 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>323</v>
+        <v>279</v>
       </c>
       <c r="D20" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E20" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="F20" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G20" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
       <c r="I20" t="s">
         <v>25</v>
@@ -2141,7 +2012,7 @@
         <v>26</v>
       </c>
       <c r="L20" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.25">
@@ -2152,19 +2023,19 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>324</v>
+        <v>280</v>
       </c>
       <c r="D21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="E21" t="s">
-        <v>72</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G21" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="I21" t="s">
         <v>25</v>
@@ -2181,13 +2052,13 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>325</v>
+        <v>281</v>
       </c>
       <c r="D22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="E22" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
@@ -2207,19 +2078,19 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>326</v>
+        <v>282</v>
       </c>
       <c r="D23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="E23" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
       <c r="F23" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="I23" t="s">
         <v>25</v>
@@ -2236,13 +2107,13 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>327</v>
+        <v>283</v>
       </c>
       <c r="D24" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="E24" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
       <c r="F24" t="s">
         <v>16</v>
@@ -2262,19 +2133,19 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>328</v>
+        <v>284</v>
       </c>
       <c r="D25" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
       <c r="F25" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G25" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I25" t="s">
         <v>25</v>
@@ -2283,7 +2154,7 @@
         <v>26</v>
       </c>
       <c r="L25" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
@@ -2294,19 +2165,19 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>329</v>
+        <v>285</v>
       </c>
       <c r="D26" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E26" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F26" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G26" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
       <c r="I26" t="s">
         <v>25</v>
@@ -2315,7 +2186,7 @@
         <v>26</v>
       </c>
       <c r="L26" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.25">
@@ -2326,19 +2197,19 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>330</v>
+        <v>286</v>
       </c>
       <c r="D27" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="E27" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
       <c r="F27" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>74</v>
       </c>
       <c r="I27" t="s">
         <v>25</v>
@@ -2347,7 +2218,7 @@
         <v>26</v>
       </c>
       <c r="L27" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.25">
@@ -2358,19 +2229,19 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>331</v>
+        <v>287</v>
       </c>
       <c r="D28" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="E28" t="s">
-        <v>86</v>
+        <v>75</v>
       </c>
       <c r="F28" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
         <v>25</v>
@@ -2379,7 +2250,7 @@
         <v>26</v>
       </c>
       <c r="L28" t="s">
-        <v>88</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.25">
@@ -2390,13 +2261,13 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>332</v>
+        <v>288</v>
       </c>
       <c r="D29" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="E29" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
@@ -2416,19 +2287,19 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>333</v>
+        <v>289</v>
       </c>
       <c r="D30" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="E30" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
       <c r="F30" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G30" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
       <c r="I30" t="s">
         <v>25</v>
@@ -2445,19 +2316,19 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>334</v>
+        <v>290</v>
       </c>
       <c r="D31" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="E31" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
       <c r="F31" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G31" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
       <c r="I31" t="s">
         <v>25</v>
@@ -2474,19 +2345,19 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>335</v>
+        <v>291</v>
       </c>
       <c r="D32" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="E32" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
       <c r="F32" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G32" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I32" t="s">
         <v>25</v>
@@ -2503,19 +2374,19 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>336</v>
+        <v>292</v>
       </c>
       <c r="D33" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="E33" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
       <c r="F33" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G33" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I33" t="s">
         <v>25</v>
@@ -2532,19 +2403,19 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>337</v>
+        <v>293</v>
       </c>
       <c r="D34" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="E34" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
       <c r="F34" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G34" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I34" t="s">
         <v>25</v>
@@ -2561,19 +2432,19 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>338</v>
+        <v>294</v>
       </c>
       <c r="D35" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="E35" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
       <c r="F35" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G35" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I35" t="s">
         <v>25</v>
@@ -2590,19 +2461,19 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>339</v>
+        <v>295</v>
       </c>
       <c r="D36" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="E36" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
       <c r="F36" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G36" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I36" t="s">
         <v>25</v>
@@ -2619,19 +2490,19 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>340</v>
+        <v>296</v>
       </c>
       <c r="D37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="E37" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
       <c r="F37" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G37" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
       <c r="I37" t="s">
         <v>25</v>
@@ -2648,19 +2519,19 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>341</v>
+        <v>297</v>
       </c>
       <c r="D38" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
       <c r="E38" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
       <c r="F38" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G38" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="I38" t="s">
         <v>25</v>
@@ -2677,13 +2548,13 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>342</v>
+        <v>298</v>
       </c>
       <c r="D39" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
       <c r="E39" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
@@ -2703,19 +2574,19 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>343</v>
+        <v>299</v>
       </c>
       <c r="D40" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="E40" t="s">
-        <v>110</v>
+        <v>97</v>
       </c>
       <c r="F40" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G40" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
       <c r="I40" t="s">
         <v>25</v>
@@ -2732,13 +2603,13 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>344</v>
+        <v>300</v>
       </c>
       <c r="D41" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E41" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
@@ -2758,19 +2629,19 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>345</v>
+        <v>301</v>
       </c>
       <c r="D42" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="E42" t="s">
-        <v>114</v>
+        <v>100</v>
       </c>
       <c r="F42" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G42" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="I42" t="s">
         <v>25</v>
@@ -2787,19 +2658,19 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>346</v>
+        <v>302</v>
       </c>
       <c r="D43" t="s">
-        <v>116</v>
+        <v>102</v>
       </c>
       <c r="E43" t="s">
-        <v>117</v>
+        <v>103</v>
       </c>
       <c r="F43" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G43" t="s">
-        <v>118</v>
+        <v>104</v>
       </c>
       <c r="I43" t="s">
         <v>25</v>
@@ -2816,13 +2687,13 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>347</v>
+        <v>303</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="E44" t="s">
-        <v>120</v>
+        <v>105</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
@@ -2842,13 +2713,13 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>348</v>
+        <v>304</v>
       </c>
       <c r="D45" t="s">
-        <v>122</v>
+        <v>106</v>
       </c>
       <c r="E45" t="s">
-        <v>123</v>
+        <v>107</v>
       </c>
       <c r="F45" t="s">
         <v>20</v>
@@ -2860,7 +2731,7 @@
         <v>26</v>
       </c>
       <c r="L45" t="s">
-        <v>124</v>
+        <v>108</v>
       </c>
     </row>
     <row r="46" spans="1:12" x14ac:dyDescent="0.25">
@@ -2871,13 +2742,13 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>349</v>
+        <v>305</v>
       </c>
       <c r="D46" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="E46" t="s">
-        <v>126</v>
+        <v>109</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
@@ -2897,19 +2768,19 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>350</v>
+        <v>306</v>
       </c>
       <c r="D47" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="E47" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="F47" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G47" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="I47" t="s">
         <v>25</v>
@@ -2926,13 +2797,13 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>351</v>
+        <v>307</v>
       </c>
       <c r="D48" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="E48" t="s">
-        <v>130</v>
+        <v>112</v>
       </c>
       <c r="F48" t="s">
         <v>20</v>
@@ -2952,13 +2823,13 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>352</v>
+        <v>308</v>
       </c>
       <c r="D49" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="E49" t="s">
-        <v>133</v>
+        <v>114</v>
       </c>
       <c r="F49" t="s">
         <v>20</v>
@@ -2970,7 +2841,7 @@
         <v>26</v>
       </c>
       <c r="L49" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="50" spans="1:12" x14ac:dyDescent="0.25">
@@ -2981,13 +2852,13 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>353</v>
+        <v>309</v>
       </c>
       <c r="D50" t="s">
-        <v>136</v>
+        <v>116</v>
       </c>
       <c r="E50" t="s">
-        <v>137</v>
+        <v>117</v>
       </c>
       <c r="F50" t="s">
         <v>20</v>
@@ -2999,7 +2870,7 @@
         <v>26</v>
       </c>
       <c r="L50" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="51" spans="1:12" x14ac:dyDescent="0.25">
@@ -3010,13 +2881,13 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>354</v>
+        <v>310</v>
       </c>
       <c r="D51" t="s">
-        <v>139</v>
+        <v>118</v>
       </c>
       <c r="E51" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="F51" t="s">
         <v>20</v>
@@ -3028,7 +2899,7 @@
         <v>26</v>
       </c>
       <c r="L51" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="52" spans="1:12" x14ac:dyDescent="0.25">
@@ -3039,13 +2910,13 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>355</v>
+        <v>311</v>
       </c>
       <c r="D52" t="s">
-        <v>142</v>
+        <v>120</v>
       </c>
       <c r="E52" t="s">
-        <v>143</v>
+        <v>121</v>
       </c>
       <c r="F52" t="s">
         <v>20</v>
@@ -3057,7 +2928,7 @@
         <v>26</v>
       </c>
       <c r="L52" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:12" x14ac:dyDescent="0.25">
@@ -3068,13 +2939,13 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>356</v>
+        <v>312</v>
       </c>
       <c r="D53" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>122</v>
       </c>
       <c r="F53" t="s">
         <v>20</v>
@@ -3086,7 +2957,7 @@
         <v>26</v>
       </c>
       <c r="L53" t="s">
-        <v>134</v>
+        <v>115</v>
       </c>
     </row>
     <row r="54" spans="1:12" x14ac:dyDescent="0.25">
@@ -3097,13 +2968,13 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>357</v>
+        <v>313</v>
       </c>
       <c r="D54" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="E54" t="s">
-        <v>147</v>
+        <v>123</v>
       </c>
       <c r="F54" t="s">
         <v>20</v>
@@ -3123,13 +2994,13 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>358</v>
+        <v>314</v>
       </c>
       <c r="D55" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="E55" t="s">
-        <v>149</v>
+        <v>124</v>
       </c>
       <c r="F55" t="s">
         <v>20</v>
@@ -3149,13 +3020,13 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>359</v>
+        <v>315</v>
       </c>
       <c r="D56" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="E56" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="F56" t="s">
         <v>20</v>
@@ -3175,13 +3046,13 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>360</v>
+        <v>316</v>
       </c>
       <c r="D57" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="E57" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="F57" t="s">
         <v>20</v>
@@ -3201,13 +3072,13 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>361</v>
+        <v>317</v>
       </c>
       <c r="D58" t="s">
-        <v>155</v>
+        <v>127</v>
       </c>
       <c r="E58" t="s">
-        <v>156</v>
+        <v>128</v>
       </c>
       <c r="F58" t="s">
         <v>20</v>
@@ -3227,13 +3098,13 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>362</v>
+        <v>318</v>
       </c>
       <c r="D59" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="E59" t="s">
-        <v>157</v>
+        <v>129</v>
       </c>
       <c r="F59" t="s">
         <v>20</v>
@@ -3253,13 +3124,13 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>363</v>
+        <v>319</v>
       </c>
       <c r="D60" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="E60" t="s">
-        <v>158</v>
+        <v>130</v>
       </c>
       <c r="F60" t="s">
         <v>20</v>
@@ -3279,13 +3150,13 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>364</v>
+        <v>320</v>
       </c>
       <c r="D61" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="E61" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="F61" t="s">
         <v>20</v>
@@ -3305,13 +3176,13 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>365</v>
+        <v>321</v>
       </c>
       <c r="D62" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="E62" t="s">
-        <v>160</v>
+        <v>132</v>
       </c>
       <c r="F62" t="s">
         <v>20</v>
@@ -3331,13 +3202,13 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>366</v>
+        <v>322</v>
       </c>
       <c r="D63" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="E63" t="s">
-        <v>161</v>
+        <v>133</v>
       </c>
       <c r="F63" t="s">
         <v>20</v>
@@ -3357,13 +3228,13 @@
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>367</v>
+        <v>323</v>
       </c>
       <c r="D64" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="E64" t="s">
-        <v>162</v>
+        <v>134</v>
       </c>
       <c r="F64" t="s">
         <v>20</v>
@@ -3383,13 +3254,13 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>368</v>
+        <v>324</v>
       </c>
       <c r="D65" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="E65" t="s">
-        <v>163</v>
+        <v>135</v>
       </c>
       <c r="F65" t="s">
         <v>20</v>
@@ -3409,13 +3280,13 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>369</v>
+        <v>325</v>
       </c>
       <c r="D66" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="E66" t="s">
-        <v>165</v>
+        <v>136</v>
       </c>
       <c r="F66" t="s">
         <v>20</v>
@@ -3435,19 +3306,19 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>370</v>
+        <v>326</v>
       </c>
       <c r="D67" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="E67" t="s">
-        <v>166</v>
+        <v>137</v>
       </c>
       <c r="F67" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="G67" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="I67" t="s">
         <v>25</v>
@@ -3464,13 +3335,13 @@
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>371</v>
+        <v>327</v>
       </c>
       <c r="D68" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="E68" t="s">
-        <v>169</v>
+        <v>139</v>
       </c>
       <c r="F68" t="s">
         <v>20</v>
@@ -3490,13 +3361,13 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>372</v>
+        <v>328</v>
       </c>
       <c r="D69" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="E69" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="F69" t="s">
         <v>20</v>
@@ -3516,13 +3387,13 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>373</v>
+        <v>329</v>
       </c>
       <c r="D70" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="E70" t="s">
-        <v>173</v>
+        <v>141</v>
       </c>
       <c r="F70" t="s">
         <v>20</v>
@@ -3534,7 +3405,7 @@
         <v>26</v>
       </c>
       <c r="L70" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.25">
@@ -3545,13 +3416,13 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>374</v>
+        <v>330</v>
       </c>
       <c r="D71" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="E71" t="s">
-        <v>176</v>
+        <v>143</v>
       </c>
       <c r="F71" t="s">
         <v>20</v>
@@ -3571,13 +3442,13 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>375</v>
+        <v>331</v>
       </c>
       <c r="D72" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="E72" t="s">
-        <v>178</v>
+        <v>144</v>
       </c>
       <c r="F72" t="s">
         <v>20</v>
@@ -3597,13 +3468,13 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>376</v>
+        <v>332</v>
       </c>
       <c r="D73" t="s">
-        <v>180</v>
+        <v>145</v>
       </c>
       <c r="E73" t="s">
-        <v>181</v>
+        <v>146</v>
       </c>
       <c r="F73" t="s">
         <v>20</v>
@@ -3623,13 +3494,13 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>377</v>
+        <v>333</v>
       </c>
       <c r="D74" t="s">
-        <v>183</v>
+        <v>147</v>
       </c>
       <c r="E74" t="s">
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="F74" t="s">
         <v>20</v>
@@ -3641,7 +3512,7 @@
         <v>26</v>
       </c>
       <c r="L74" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.25">
@@ -3652,13 +3523,13 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>378</v>
+        <v>334</v>
       </c>
       <c r="D75" t="s">
-        <v>186</v>
+        <v>149</v>
       </c>
       <c r="E75" t="s">
-        <v>187</v>
+        <v>150</v>
       </c>
       <c r="F75" t="s">
         <v>20</v>
@@ -3670,7 +3541,7 @@
         <v>26</v>
       </c>
       <c r="L75" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.25">
@@ -3681,19 +3552,19 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>379</v>
+        <v>335</v>
       </c>
       <c r="D76" t="s">
-        <v>188</v>
+        <v>151</v>
       </c>
       <c r="E76" t="s">
-        <v>189</v>
+        <v>152</v>
       </c>
       <c r="F76" t="s">
         <v>20</v>
       </c>
       <c r="G76" t="s">
-        <v>167</v>
+        <v>138</v>
       </c>
       <c r="I76" t="s">
         <v>25</v>
@@ -3702,7 +3573,7 @@
         <v>26</v>
       </c>
       <c r="L76" t="s">
-        <v>174</v>
+        <v>142</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.25">
@@ -3713,13 +3584,13 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>380</v>
+        <v>336</v>
       </c>
       <c r="D77" t="s">
-        <v>191</v>
+        <v>153</v>
       </c>
       <c r="E77" t="s">
-        <v>192</v>
+        <v>154</v>
       </c>
       <c r="F77" t="s">
         <v>20</v>
@@ -3739,13 +3610,13 @@
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>381</v>
+        <v>337</v>
       </c>
       <c r="D78" t="s">
-        <v>194</v>
+        <v>155</v>
       </c>
       <c r="E78" t="s">
-        <v>195</v>
+        <v>156</v>
       </c>
       <c r="F78" t="s">
         <v>20</v>
@@ -3765,13 +3636,13 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>382</v>
+        <v>338</v>
       </c>
       <c r="D79" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="E79" t="s">
-        <v>197</v>
+        <v>157</v>
       </c>
       <c r="F79" t="s">
         <v>20</v>
@@ -3791,13 +3662,13 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>383</v>
+        <v>339</v>
       </c>
       <c r="D80" t="s">
-        <v>199</v>
+        <v>158</v>
       </c>
       <c r="E80" t="s">
-        <v>200</v>
+        <v>159</v>
       </c>
       <c r="F80" t="s">
         <v>20</v>
@@ -3809,7 +3680,7 @@
         <v>26</v>
       </c>
       <c r="L80" t="s">
-        <v>201</v>
+        <v>160</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -3820,13 +3691,13 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>384</v>
+        <v>340</v>
       </c>
       <c r="D81" t="s">
-        <v>203</v>
+        <v>161</v>
       </c>
       <c r="E81" t="s">
-        <v>204</v>
+        <v>162</v>
       </c>
       <c r="F81" t="s">
         <v>20</v>
@@ -3846,13 +3717,13 @@
         <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>385</v>
+        <v>341</v>
       </c>
       <c r="D82" t="s">
-        <v>206</v>
+        <v>163</v>
       </c>
       <c r="E82" t="s">
-        <v>207</v>
+        <v>164</v>
       </c>
       <c r="F82" t="s">
         <v>20</v>
@@ -3864,7 +3735,7 @@
         <v>26</v>
       </c>
       <c r="L82" t="s">
-        <v>208</v>
+        <v>165</v>
       </c>
     </row>
     <row r="83" spans="1:12" x14ac:dyDescent="0.25">
@@ -3875,16 +3746,16 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>386</v>
+        <v>342</v>
       </c>
       <c r="D83" t="s">
-        <v>209</v>
+        <v>166</v>
       </c>
       <c r="E83" t="s">
-        <v>210</v>
+        <v>167</v>
       </c>
       <c r="F83" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I83" t="s">
         <v>25</v>
@@ -3901,19 +3772,19 @@
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>387</v>
+        <v>343</v>
       </c>
       <c r="D84" t="s">
-        <v>211</v>
+        <v>168</v>
       </c>
       <c r="E84" t="s">
-        <v>212</v>
+        <v>169</v>
       </c>
       <c r="F84" t="s">
         <v>20</v>
       </c>
       <c r="G84" t="s">
-        <v>213</v>
+        <v>170</v>
       </c>
       <c r="I84" t="s">
         <v>25</v>
@@ -3931,8 +3802,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0F4D0D-50C6-45AA-88F3-85EA0E56D506}">
   <dimension ref="A1:F129"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3944,16 +3815,16 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>215</v>
+        <v>171</v>
       </c>
       <c r="B1" t="s">
-        <v>216</v>
+        <v>172</v>
       </c>
       <c r="C1" t="s">
-        <v>217</v>
+        <v>173</v>
       </c>
       <c r="D1" t="s">
-        <v>218</v>
+        <v>174</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -3967,7 +3838,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>27</v>
+        <v>264</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3976,7 +3847,7 @@
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>219</v>
+        <v>175</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -3984,7 +3855,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>27</v>
+        <v>264</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3993,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>220</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -4001,7 +3872,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -4010,7 +3881,7 @@
         <v>0</v>
       </c>
       <c r="F4" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -4018,7 +3889,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -4027,7 +3898,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>222</v>
+        <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -4035,7 +3906,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -4044,7 +3915,7 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>223</v>
+        <v>179</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -4052,7 +3923,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>33</v>
+        <v>266</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -4061,7 +3932,7 @@
         <v>3</v>
       </c>
       <c r="F7" t="s">
-        <v>224</v>
+        <v>180</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -4069,7 +3940,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>36</v>
+        <v>267</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -4078,7 +3949,7 @@
         <v>0</v>
       </c>
       <c r="F8" t="s">
-        <v>225</v>
+        <v>181</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -4086,7 +3957,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>36</v>
+        <v>267</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -4095,7 +3966,7 @@
         <v>1</v>
       </c>
       <c r="F9" t="s">
-        <v>226</v>
+        <v>182</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -4103,7 +3974,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>49</v>
+        <v>271</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -4112,7 +3983,7 @@
         <v>0</v>
       </c>
       <c r="F10" t="s">
-        <v>227</v>
+        <v>183</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -4120,7 +3991,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>49</v>
+        <v>271</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -4129,7 +4000,7 @@
         <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>228</v>
+        <v>184</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -4137,7 +4008,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>268</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -4146,7 +4017,7 @@
         <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>229</v>
+        <v>185</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -4154,7 +4025,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>268</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4163,7 +4034,7 @@
         <v>2</v>
       </c>
       <c r="F13" t="s">
-        <v>230</v>
+        <v>186</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -4171,7 +4042,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -4180,7 +4051,7 @@
         <v>0</v>
       </c>
       <c r="F14" t="s">
-        <v>231</v>
+        <v>187</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -4188,7 +4059,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -4197,7 +4068,7 @@
         <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>232</v>
+        <v>188</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -4205,7 +4076,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>53</v>
+        <v>272</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4214,7 +4085,7 @@
         <v>2</v>
       </c>
       <c r="F16" t="s">
-        <v>233</v>
+        <v>189</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -4222,7 +4093,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>56</v>
+        <v>273</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4231,7 +4102,7 @@
         <v>0</v>
       </c>
       <c r="F17" t="s">
-        <v>234</v>
+        <v>190</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -4239,7 +4110,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>56</v>
+        <v>273</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4248,7 +4119,7 @@
         <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>235</v>
+        <v>191</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -4256,7 +4127,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>59</v>
+        <v>274</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4265,7 +4136,7 @@
         <v>1</v>
       </c>
       <c r="F19" t="s">
-        <v>236</v>
+        <v>192</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -4273,7 +4144,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>59</v>
+        <v>274</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4282,7 +4153,7 @@
         <v>2</v>
       </c>
       <c r="F20" t="s">
-        <v>237</v>
+        <v>193</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -4290,7 +4161,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>63</v>
+        <v>276</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4299,7 +4170,7 @@
         <v>1</v>
       </c>
       <c r="F21" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -4307,7 +4178,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>63</v>
+        <v>276</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4316,7 +4187,7 @@
         <v>2</v>
       </c>
       <c r="F22" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -4324,7 +4195,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>67</v>
+        <v>278</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4333,7 +4204,7 @@
         <v>1</v>
       </c>
       <c r="F23" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -4341,7 +4212,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>67</v>
+        <v>278</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4350,7 +4221,7 @@
         <v>2</v>
       </c>
       <c r="F24" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -4358,7 +4229,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>73</v>
+        <v>281</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4367,7 +4238,7 @@
         <v>1</v>
       </c>
       <c r="F25" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -4375,7 +4246,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>73</v>
+        <v>281</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4384,7 +4255,7 @@
         <v>2</v>
       </c>
       <c r="F26" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -4392,7 +4263,7 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>89</v>
+        <v>288</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4401,7 +4272,7 @@
         <v>0</v>
       </c>
       <c r="F27" t="s">
-        <v>240</v>
+        <v>196</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -4409,7 +4280,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>89</v>
+        <v>288</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -4418,7 +4289,7 @@
         <v>1</v>
       </c>
       <c r="F28" t="s">
-        <v>241</v>
+        <v>197</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -4426,7 +4297,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>89</v>
+        <v>288</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4435,7 +4306,7 @@
         <v>2</v>
       </c>
       <c r="F29" t="s">
-        <v>242</v>
+        <v>198</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -4443,7 +4314,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4452,7 +4323,7 @@
         <v>1</v>
       </c>
       <c r="F30" t="s">
-        <v>243</v>
+        <v>199</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -4460,7 +4331,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4469,7 +4340,7 @@
         <v>2</v>
       </c>
       <c r="F31" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -4477,7 +4348,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>298</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4486,7 +4357,7 @@
         <v>3</v>
       </c>
       <c r="F32" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -4494,7 +4365,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -4503,7 +4374,7 @@
         <v>1</v>
       </c>
       <c r="F33" t="s">
-        <v>243</v>
+        <v>199</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -4511,7 +4382,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -4520,7 +4391,7 @@
         <v>2</v>
       </c>
       <c r="F34" t="s">
-        <v>244</v>
+        <v>200</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -4528,7 +4399,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>111</v>
+        <v>300</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -4537,7 +4408,7 @@
         <v>3</v>
       </c>
       <c r="F35" t="s">
-        <v>245</v>
+        <v>201</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -4545,7 +4416,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4554,7 +4425,7 @@
         <v>0</v>
       </c>
       <c r="F36" t="s">
-        <v>246</v>
+        <v>202</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -4562,7 +4433,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -4571,7 +4442,7 @@
         <v>1</v>
       </c>
       <c r="F37" t="s">
-        <v>247</v>
+        <v>203</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -4579,7 +4450,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -4588,7 +4459,7 @@
         <v>2</v>
       </c>
       <c r="F38" t="s">
-        <v>248</v>
+        <v>204</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -4596,7 +4467,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>119</v>
+        <v>303</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -4605,7 +4476,7 @@
         <v>3</v>
       </c>
       <c r="F39" t="s">
-        <v>249</v>
+        <v>205</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -4613,7 +4484,7 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4622,7 +4493,7 @@
         <v>0</v>
       </c>
       <c r="F40" t="s">
-        <v>250</v>
+        <v>206</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -4630,7 +4501,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -4639,7 +4510,7 @@
         <v>1</v>
       </c>
       <c r="F41" t="s">
-        <v>251</v>
+        <v>207</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -4647,7 +4518,7 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>121</v>
+        <v>304</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -4656,7 +4527,7 @@
         <v>2</v>
       </c>
       <c r="F42" t="s">
-        <v>252</v>
+        <v>208</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -4664,7 +4535,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>125</v>
+        <v>305</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -4673,7 +4544,7 @@
         <v>1</v>
       </c>
       <c r="F43" t="s">
-        <v>253</v>
+        <v>209</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -4681,7 +4552,7 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>125</v>
+        <v>305</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -4690,7 +4561,7 @@
         <v>2</v>
       </c>
       <c r="F44" t="s">
-        <v>249</v>
+        <v>205</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -4698,7 +4569,7 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -4707,7 +4578,7 @@
         <v>1</v>
       </c>
       <c r="F45" t="s">
-        <v>254</v>
+        <v>210</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -4715,7 +4586,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4724,7 +4595,7 @@
         <v>2</v>
       </c>
       <c r="F46" t="s">
-        <v>255</v>
+        <v>211</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -4732,7 +4603,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4741,7 +4612,7 @@
         <v>3</v>
       </c>
       <c r="F47" t="s">
-        <v>256</v>
+        <v>212</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -4749,7 +4620,7 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>129</v>
+        <v>307</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4758,7 +4629,7 @@
         <v>4</v>
       </c>
       <c r="F48" t="s">
-        <v>257</v>
+        <v>213</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -4766,7 +4637,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>131</v>
+        <v>308</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4775,7 +4646,7 @@
         <v>0</v>
       </c>
       <c r="F49" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -4783,7 +4654,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>131</v>
+        <v>308</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4792,7 +4663,7 @@
         <v>1</v>
       </c>
       <c r="F50" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -4800,7 +4671,7 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>135</v>
+        <v>309</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4809,7 +4680,7 @@
         <v>0</v>
       </c>
       <c r="F51" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -4817,7 +4688,7 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>135</v>
+        <v>309</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4826,7 +4697,7 @@
         <v>1</v>
       </c>
       <c r="F52" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -4834,7 +4705,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>138</v>
+        <v>310</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4843,7 +4714,7 @@
         <v>0</v>
       </c>
       <c r="F53" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -4851,7 +4722,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>138</v>
+        <v>310</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4860,7 +4731,7 @@
         <v>1</v>
       </c>
       <c r="F54" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -4868,7 +4739,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>141</v>
+        <v>311</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4877,7 +4748,7 @@
         <v>1</v>
       </c>
       <c r="F55" t="s">
-        <v>260</v>
+        <v>216</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -4885,7 +4756,7 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>141</v>
+        <v>311</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4894,7 +4765,7 @@
         <v>2</v>
       </c>
       <c r="F56" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -4902,7 +4773,7 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>141</v>
+        <v>311</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4911,7 +4782,7 @@
         <v>3</v>
       </c>
       <c r="F57" t="s">
-        <v>262</v>
+        <v>218</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -4919,7 +4790,7 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4928,7 +4799,7 @@
         <v>0</v>
       </c>
       <c r="F58" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -4936,7 +4807,7 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>144</v>
+        <v>312</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4945,7 +4816,7 @@
         <v>1</v>
       </c>
       <c r="F59" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -4953,7 +4824,7 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>146</v>
+        <v>313</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4962,7 +4833,7 @@
         <v>0</v>
       </c>
       <c r="F60" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -4970,7 +4841,7 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>146</v>
+        <v>313</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4979,7 +4850,7 @@
         <v>1</v>
       </c>
       <c r="F61" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -4987,7 +4858,7 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>148</v>
+        <v>314</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4996,7 +4867,7 @@
         <v>0</v>
       </c>
       <c r="F62" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -5004,7 +4875,7 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>148</v>
+        <v>314</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -5013,7 +4884,7 @@
         <v>1</v>
       </c>
       <c r="F63" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -5021,7 +4892,7 @@
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>150</v>
+        <v>315</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -5030,7 +4901,7 @@
         <v>0</v>
       </c>
       <c r="F64" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -5038,7 +4909,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>150</v>
+        <v>315</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -5047,7 +4918,7 @@
         <v>1</v>
       </c>
       <c r="F65" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -5055,7 +4926,7 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -5064,7 +4935,7 @@
         <v>0</v>
       </c>
       <c r="F66" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -5072,7 +4943,7 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>152</v>
+        <v>316</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -5081,7 +4952,7 @@
         <v>1</v>
       </c>
       <c r="F67" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -5089,7 +4960,7 @@
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>154</v>
+        <v>317</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -5098,7 +4969,7 @@
         <v>0</v>
       </c>
       <c r="F68" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -5106,7 +4977,7 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>154</v>
+        <v>317</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -5115,7 +4986,7 @@
         <v>1</v>
       </c>
       <c r="F69" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -5123,7 +4994,7 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>164</v>
+        <v>325</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -5132,7 +5003,7 @@
         <v>0</v>
       </c>
       <c r="F70" t="s">
-        <v>263</v>
+        <v>219</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -5140,7 +5011,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>164</v>
+        <v>325</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -5149,7 +5020,7 @@
         <v>1</v>
       </c>
       <c r="F71" t="s">
-        <v>264</v>
+        <v>220</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -5157,7 +5028,7 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -5166,7 +5037,7 @@
         <v>1</v>
       </c>
       <c r="F72" t="s">
-        <v>265</v>
+        <v>221</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -5174,7 +5045,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -5183,7 +5054,7 @@
         <v>2</v>
       </c>
       <c r="F73" t="s">
-        <v>266</v>
+        <v>222</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -5191,7 +5062,7 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -5200,7 +5071,7 @@
         <v>3</v>
       </c>
       <c r="F74" t="s">
-        <v>267</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -5208,7 +5079,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5217,7 +5088,7 @@
         <v>4</v>
       </c>
       <c r="F75" t="s">
-        <v>268</v>
+        <v>224</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -5225,7 +5096,7 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5234,7 +5105,7 @@
         <v>5</v>
       </c>
       <c r="F76" t="s">
-        <v>269</v>
+        <v>225</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -5242,7 +5113,7 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5251,7 +5122,7 @@
         <v>6</v>
       </c>
       <c r="F77" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -5259,7 +5130,7 @@
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5268,7 +5139,7 @@
         <v>7</v>
       </c>
       <c r="F78" t="s">
-        <v>271</v>
+        <v>227</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -5276,7 +5147,7 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5285,7 +5156,7 @@
         <v>8</v>
       </c>
       <c r="F79" t="s">
-        <v>272</v>
+        <v>228</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -5293,7 +5164,7 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>168</v>
+        <v>327</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5302,7 +5173,7 @@
         <v>9</v>
       </c>
       <c r="F80" t="s">
-        <v>273</v>
+        <v>229</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -5310,7 +5181,7 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>170</v>
+        <v>328</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5319,7 +5190,7 @@
         <v>0</v>
       </c>
       <c r="F81" t="s">
-        <v>274</v>
+        <v>230</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,7 +5198,7 @@
         <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>170</v>
+        <v>328</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5336,7 +5207,7 @@
         <v>1</v>
       </c>
       <c r="F82" t="s">
-        <v>275</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -5344,7 +5215,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5353,7 +5224,7 @@
         <v>1</v>
       </c>
       <c r="F83" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -5361,7 +5232,7 @@
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5370,7 +5241,7 @@
         <v>2</v>
       </c>
       <c r="F84" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -5378,7 +5249,7 @@
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>172</v>
+        <v>329</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5387,7 +5258,7 @@
         <v>3</v>
       </c>
       <c r="F85" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -5395,7 +5266,7 @@
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>175</v>
+        <v>330</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5404,7 +5275,7 @@
         <v>1</v>
       </c>
       <c r="F86" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -5412,7 +5283,7 @@
         <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>175</v>
+        <v>330</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5421,7 +5292,7 @@
         <v>2</v>
       </c>
       <c r="F87" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -5429,7 +5300,7 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>175</v>
+        <v>330</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5438,7 +5309,7 @@
         <v>3</v>
       </c>
       <c r="F88" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -5446,7 +5317,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5455,7 +5326,7 @@
         <v>1</v>
       </c>
       <c r="F89" t="s">
-        <v>276</v>
+        <v>232</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -5463,7 +5334,7 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5472,7 +5343,7 @@
         <v>2</v>
       </c>
       <c r="F90" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -5480,7 +5351,7 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>177</v>
+        <v>331</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5489,7 +5360,7 @@
         <v>3</v>
       </c>
       <c r="F91" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -5497,7 +5368,7 @@
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5506,7 +5377,7 @@
         <v>1</v>
       </c>
       <c r="F92" t="s">
-        <v>279</v>
+        <v>235</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -5514,7 +5385,7 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5523,7 +5394,7 @@
         <v>2</v>
       </c>
       <c r="F93" t="s">
-        <v>280</v>
+        <v>236</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -5531,7 +5402,7 @@
         <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5540,7 +5411,7 @@
         <v>3</v>
       </c>
       <c r="F94" t="s">
-        <v>281</v>
+        <v>237</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -5548,7 +5419,7 @@
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5557,7 +5428,7 @@
         <v>4</v>
       </c>
       <c r="F95" t="s">
-        <v>282</v>
+        <v>238</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -5565,7 +5436,7 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5574,7 +5445,7 @@
         <v>5</v>
       </c>
       <c r="F96" t="s">
-        <v>283</v>
+        <v>239</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -5582,7 +5453,7 @@
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -5591,7 +5462,7 @@
         <v>6</v>
       </c>
       <c r="F97" t="s">
-        <v>284</v>
+        <v>240</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -5599,7 +5470,7 @@
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -5608,7 +5479,7 @@
         <v>7</v>
       </c>
       <c r="F98" t="s">
-        <v>285</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -5616,7 +5487,7 @@
         <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5625,7 +5496,7 @@
         <v>8</v>
       </c>
       <c r="F99" t="s">
-        <v>286</v>
+        <v>242</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -5633,7 +5504,7 @@
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5642,7 +5513,7 @@
         <v>9</v>
       </c>
       <c r="F100" t="s">
-        <v>287</v>
+        <v>243</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -5650,7 +5521,7 @@
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5659,7 +5530,7 @@
         <v>10</v>
       </c>
       <c r="F101" t="s">
-        <v>288</v>
+        <v>244</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -5667,7 +5538,7 @@
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>179</v>
+        <v>332</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5676,7 +5547,7 @@
         <v>11</v>
       </c>
       <c r="F102" t="s">
-        <v>289</v>
+        <v>245</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -5684,7 +5555,7 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5693,7 +5564,7 @@
         <v>1</v>
       </c>
       <c r="F103" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -5701,7 +5572,7 @@
         <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5710,7 +5581,7 @@
         <v>2</v>
       </c>
       <c r="F104" t="s">
-        <v>291</v>
+        <v>247</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -5718,7 +5589,7 @@
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>182</v>
+        <v>333</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -5727,7 +5598,7 @@
         <v>3</v>
       </c>
       <c r="F105" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -5735,7 +5606,7 @@
         <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>185</v>
+        <v>334</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5744,7 +5615,7 @@
         <v>1</v>
       </c>
       <c r="F106" t="s">
-        <v>292</v>
+        <v>248</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -5752,7 +5623,7 @@
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>185</v>
+        <v>334</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5761,7 +5632,7 @@
         <v>2</v>
       </c>
       <c r="F107" t="s">
-        <v>277</v>
+        <v>233</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -5769,7 +5640,7 @@
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>185</v>
+        <v>334</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5778,7 +5649,7 @@
         <v>3</v>
       </c>
       <c r="F108" t="s">
-        <v>278</v>
+        <v>234</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -5786,7 +5657,7 @@
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5795,7 +5666,7 @@
         <v>0</v>
       </c>
       <c r="F109" t="s">
-        <v>293</v>
+        <v>249</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -5803,7 +5674,7 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5812,7 +5683,7 @@
         <v>1</v>
       </c>
       <c r="F110" t="s">
-        <v>290</v>
+        <v>246</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -5820,7 +5691,7 @@
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5829,7 +5700,7 @@
         <v>2</v>
       </c>
       <c r="F111" t="s">
-        <v>294</v>
+        <v>250</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -5837,7 +5708,7 @@
         <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5846,7 +5717,7 @@
         <v>3</v>
       </c>
       <c r="F112" t="s">
-        <v>295</v>
+        <v>251</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -5854,7 +5725,7 @@
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -5863,7 +5734,7 @@
         <v>4</v>
       </c>
       <c r="F113" t="s">
-        <v>296</v>
+        <v>252</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -5871,7 +5742,7 @@
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>190</v>
+        <v>336</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -5880,7 +5751,7 @@
         <v>5</v>
       </c>
       <c r="F114" t="s">
-        <v>297</v>
+        <v>253</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -5888,7 +5759,7 @@
         <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>193</v>
+        <v>337</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -5897,7 +5768,7 @@
         <v>1</v>
       </c>
       <c r="F115" t="s">
-        <v>298</v>
+        <v>254</v>
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
@@ -5905,7 +5776,7 @@
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>193</v>
+        <v>337</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5914,7 +5785,7 @@
         <v>2</v>
       </c>
       <c r="F116" t="s">
-        <v>299</v>
+        <v>255</v>
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
@@ -5922,7 +5793,7 @@
         <v>12</v>
       </c>
       <c r="C117" t="s">
-        <v>193</v>
+        <v>337</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -5931,7 +5802,7 @@
         <v>3</v>
       </c>
       <c r="F117" t="s">
-        <v>300</v>
+        <v>256</v>
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
@@ -5939,7 +5810,7 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>196</v>
+        <v>338</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -5948,7 +5819,7 @@
         <v>1</v>
       </c>
       <c r="F118" t="s">
-        <v>301</v>
+        <v>257</v>
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
@@ -5956,7 +5827,7 @@
         <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>196</v>
+        <v>338</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -5965,7 +5836,7 @@
         <v>2</v>
       </c>
       <c r="F119" t="s">
-        <v>302</v>
+        <v>258</v>
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
@@ -5973,7 +5844,7 @@
         <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>196</v>
+        <v>338</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -5982,7 +5853,7 @@
         <v>3</v>
       </c>
       <c r="F120" t="s">
-        <v>303</v>
+        <v>259</v>
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
@@ -5990,7 +5861,7 @@
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>196</v>
+        <v>338</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -5999,7 +5870,7 @@
         <v>4</v>
       </c>
       <c r="F121" t="s">
-        <v>304</v>
+        <v>260</v>
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
@@ -6007,7 +5878,7 @@
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>198</v>
+        <v>339</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -6016,7 +5887,7 @@
         <v>0</v>
       </c>
       <c r="F122" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
@@ -6024,7 +5895,7 @@
         <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>198</v>
+        <v>339</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -6033,7 +5904,7 @@
         <v>1</v>
       </c>
       <c r="F123" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
@@ -6041,7 +5912,7 @@
         <v>12</v>
       </c>
       <c r="C124" t="s">
-        <v>202</v>
+        <v>340</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -6050,7 +5921,7 @@
         <v>0</v>
       </c>
       <c r="F124" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
@@ -6058,7 +5929,7 @@
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>202</v>
+        <v>340</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -6067,7 +5938,7 @@
         <v>1</v>
       </c>
       <c r="F125" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
@@ -6075,7 +5946,7 @@
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>205</v>
+        <v>341</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -6084,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="F126" t="s">
-        <v>258</v>
+        <v>214</v>
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
@@ -6092,7 +5963,7 @@
         <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>205</v>
+        <v>341</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -6101,7 +5972,7 @@
         <v>1</v>
       </c>
       <c r="F127" t="s">
-        <v>259</v>
+        <v>215</v>
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
@@ -6109,7 +5980,7 @@
         <v>12</v>
       </c>
       <c r="C128" t="s">
-        <v>214</v>
+        <v>344</v>
       </c>
       <c r="D128">
         <v>0</v>
@@ -6118,7 +5989,7 @@
         <v>0</v>
       </c>
       <c r="F128" t="s">
-        <v>305</v>
+        <v>261</v>
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
@@ -6126,7 +5997,7 @@
         <v>12</v>
       </c>
       <c r="C129" t="s">
-        <v>214</v>
+        <v>344</v>
       </c>
       <c r="D129">
         <v>0</v>
@@ -6135,7 +6006,7 @@
         <v>1</v>
       </c>
       <c r="F129" t="s">
-        <v>306</v>
+        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove death from categories longitudinal
</commit_message>
<xml_diff>
--- a/longitudinal/dataschema_ProPASS_longitudinal.xlsx
+++ b/longitudinal/dataschema_ProPASS_longitudinal.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lindsey\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A57A83-01E7-4581-808B-02234F5270F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1E94290-ECB2-4C36-921D-16BC7453E2A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{FC4A5C44-0DEC-4188-833A-37731883B462}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FC4A5C44-0DEC-4188-833A-37731883B462}"/>
   </bookViews>
   <sheets>
     <sheet name="Variables" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1027" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1021" uniqueCount="342">
   <si>
     <t>index</t>
   </si>
@@ -822,12 +822,6 @@
     <t>Strenuous physical work</t>
   </si>
   <si>
-    <t>Living</t>
-  </si>
-  <si>
-    <t>Deceased</t>
-  </si>
-  <si>
     <t>adm_date</t>
   </si>
   <si>
@@ -1069,9 +1063,6 @@
   </si>
   <si>
     <t>phy_SF36_nb_items</t>
-  </si>
-  <si>
-    <t>death_status</t>
   </si>
 </sst>
 </file>
@@ -1445,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{138A0E81-F778-497B-A6EC-B26BAFD348B9}">
   <dimension ref="A1:L84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1554,7 +1545,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="D4" t="s">
         <v>21</v>
@@ -1583,7 +1574,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D5" t="s">
         <v>27</v>
@@ -1609,7 +1600,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="D6" t="s">
         <v>29</v>
@@ -1638,7 +1629,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D7" t="s">
         <v>32</v>
@@ -1664,7 +1655,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8" t="s">
         <v>34</v>
@@ -1693,7 +1684,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D9" t="s">
         <v>37</v>
@@ -1722,7 +1713,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="D10" t="s">
         <v>40</v>
@@ -1748,7 +1739,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="D11" t="s">
         <v>43</v>
@@ -1774,7 +1765,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D12" t="s">
         <v>45</v>
@@ -1803,7 +1794,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D13" t="s">
         <v>48</v>
@@ -1829,7 +1820,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D14" t="s">
         <v>50</v>
@@ -1855,7 +1846,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D15" t="s">
         <v>52</v>
@@ -1881,7 +1872,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="D16" t="s">
         <v>53</v>
@@ -1910,7 +1901,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D17" t="s">
         <v>55</v>
@@ -1936,7 +1927,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="D18" t="s">
         <v>56</v>
@@ -1965,7 +1956,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D19" t="s">
         <v>58</v>
@@ -1991,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="D20" t="s">
         <v>59</v>
@@ -2023,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="D21" t="s">
         <v>62</v>
@@ -2052,7 +2043,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D22" t="s">
         <v>63</v>
@@ -2078,7 +2069,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
       <c r="D23" t="s">
         <v>64</v>
@@ -2107,7 +2098,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
       <c r="D24" t="s">
         <v>66</v>
@@ -2133,7 +2124,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="D25" t="s">
         <v>67</v>
@@ -2165,7 +2156,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="D26" t="s">
         <v>71</v>
@@ -2197,7 +2188,7 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="D27" t="s">
         <v>73</v>
@@ -2229,7 +2220,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="D28" t="s">
         <v>75</v>
@@ -2261,7 +2252,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D29" t="s">
         <v>78</v>
@@ -2287,7 +2278,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="D30" t="s">
         <v>79</v>
@@ -2316,7 +2307,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="D31" t="s">
         <v>81</v>
@@ -2345,7 +2336,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="D32" t="s">
         <v>83</v>
@@ -2374,7 +2365,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="D33" t="s">
         <v>85</v>
@@ -2403,7 +2394,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="D34" t="s">
         <v>86</v>
@@ -2432,7 +2423,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="D35" t="s">
         <v>87</v>
@@ -2461,7 +2452,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="D36" t="s">
         <v>88</v>
@@ -2490,7 +2481,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="D37" t="s">
         <v>89</v>
@@ -2519,7 +2510,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="D38" t="s">
         <v>91</v>
@@ -2548,7 +2539,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D39" t="s">
         <v>94</v>
@@ -2574,7 +2565,7 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
       <c r="D40" t="s">
         <v>96</v>
@@ -2603,7 +2594,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D41" t="s">
         <v>98</v>
@@ -2629,7 +2620,7 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="D42" t="s">
         <v>100</v>
@@ -2658,7 +2649,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="D43" t="s">
         <v>102</v>
@@ -2687,7 +2678,7 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D44" t="s">
         <v>105</v>
@@ -2713,7 +2704,7 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D45" t="s">
         <v>106</v>
@@ -2742,7 +2733,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D46" t="s">
         <v>109</v>
@@ -2768,7 +2759,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
       <c r="D47" t="s">
         <v>110</v>
@@ -2797,7 +2788,7 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D48" t="s">
         <v>112</v>
@@ -2823,7 +2814,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D49" t="s">
         <v>113</v>
@@ -2852,7 +2843,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D50" t="s">
         <v>116</v>
@@ -2881,7 +2872,7 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D51" t="s">
         <v>118</v>
@@ -2910,7 +2901,7 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D52" t="s">
         <v>120</v>
@@ -2939,7 +2930,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D53" t="s">
         <v>122</v>
@@ -2968,7 +2959,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D54" t="s">
         <v>123</v>
@@ -2994,7 +2985,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D55" t="s">
         <v>124</v>
@@ -3020,7 +3011,7 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D56" t="s">
         <v>125</v>
@@ -3046,7 +3037,7 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D57" t="s">
         <v>126</v>
@@ -3072,7 +3063,7 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D58" t="s">
         <v>127</v>
@@ -3098,7 +3089,7 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="D59" t="s">
         <v>129</v>
@@ -3124,7 +3115,7 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="D60" t="s">
         <v>130</v>
@@ -3150,7 +3141,7 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="D61" t="s">
         <v>131</v>
@@ -3176,7 +3167,7 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="D62" t="s">
         <v>132</v>
@@ -3202,7 +3193,7 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="D63" t="s">
         <v>133</v>
@@ -3228,7 +3219,7 @@
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="D64" t="s">
         <v>134</v>
@@ -3254,7 +3245,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="D65" t="s">
         <v>135</v>
@@ -3280,7 +3271,7 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D66" t="s">
         <v>136</v>
@@ -3306,7 +3297,7 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="D67" t="s">
         <v>137</v>
@@ -3335,7 +3326,7 @@
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D68" t="s">
         <v>139</v>
@@ -3361,7 +3352,7 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D69" t="s">
         <v>140</v>
@@ -3387,7 +3378,7 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D70" t="s">
         <v>141</v>
@@ -3416,7 +3407,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D71" t="s">
         <v>143</v>
@@ -3442,7 +3433,7 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D72" t="s">
         <v>144</v>
@@ -3468,7 +3459,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D73" t="s">
         <v>145</v>
@@ -3494,7 +3485,7 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D74" t="s">
         <v>147</v>
@@ -3523,7 +3514,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D75" t="s">
         <v>149</v>
@@ -3552,7 +3543,7 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="D76" t="s">
         <v>151</v>
@@ -3584,7 +3575,7 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D77" t="s">
         <v>153</v>
@@ -3610,7 +3601,7 @@
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D78" t="s">
         <v>155</v>
@@ -3636,7 +3627,7 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D79" t="s">
         <v>157</v>
@@ -3662,7 +3653,7 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D80" t="s">
         <v>158</v>
@@ -3691,7 +3682,7 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D81" t="s">
         <v>161</v>
@@ -3717,7 +3708,7 @@
         <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D82" t="s">
         <v>163</v>
@@ -3746,7 +3737,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="D83" t="s">
         <v>166</v>
@@ -3772,7 +3763,7 @@
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D84" t="s">
         <v>168</v>
@@ -3800,10 +3791,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE0F4D0D-50C6-45AA-88F3-85EA0E56D506}">
-  <dimension ref="A1:F129"/>
+  <dimension ref="A1:F127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView topLeftCell="A102" workbookViewId="0">
+      <selection activeCell="A128" sqref="A128:F129"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3838,7 +3829,7 @@
         <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D2">
         <v>0</v>
@@ -3855,7 +3846,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -3872,7 +3863,7 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D4">
         <v>0</v>
@@ -3889,7 +3880,7 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -3906,7 +3897,7 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D6">
         <v>0</v>
@@ -3923,7 +3914,7 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="D7">
         <v>0</v>
@@ -3940,7 +3931,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D8">
         <v>0</v>
@@ -3957,7 +3948,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="D9">
         <v>0</v>
@@ -3974,7 +3965,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D10">
         <v>0</v>
@@ -3991,7 +3982,7 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="D11">
         <v>0</v>
@@ -4008,7 +3999,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D12">
         <v>0</v>
@@ -4025,7 +4016,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="D13">
         <v>0</v>
@@ -4042,7 +4033,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D14">
         <v>0</v>
@@ -4059,7 +4050,7 @@
         <v>12</v>
       </c>
       <c r="C15" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D15">
         <v>0</v>
@@ -4076,7 +4067,7 @@
         <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D16">
         <v>0</v>
@@ -4093,7 +4084,7 @@
         <v>12</v>
       </c>
       <c r="C17" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D17">
         <v>0</v>
@@ -4110,7 +4101,7 @@
         <v>12</v>
       </c>
       <c r="C18" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D18">
         <v>0</v>
@@ -4127,7 +4118,7 @@
         <v>12</v>
       </c>
       <c r="C19" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D19">
         <v>0</v>
@@ -4144,7 +4135,7 @@
         <v>12</v>
       </c>
       <c r="C20" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="D20">
         <v>0</v>
@@ -4161,7 +4152,7 @@
         <v>12</v>
       </c>
       <c r="C21" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D21">
         <v>0</v>
@@ -4178,7 +4169,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="D22">
         <v>0</v>
@@ -4195,7 +4186,7 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D23">
         <v>0</v>
@@ -4212,7 +4203,7 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="D24">
         <v>0</v>
@@ -4229,7 +4220,7 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D25">
         <v>0</v>
@@ -4246,7 +4237,7 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="D26">
         <v>0</v>
@@ -4263,7 +4254,7 @@
         <v>12</v>
       </c>
       <c r="C27" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D27">
         <v>0</v>
@@ -4280,7 +4271,7 @@
         <v>12</v>
       </c>
       <c r="C28" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D28">
         <v>0</v>
@@ -4297,7 +4288,7 @@
         <v>12</v>
       </c>
       <c r="C29" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="D29">
         <v>0</v>
@@ -4314,7 +4305,7 @@
         <v>12</v>
       </c>
       <c r="C30" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D30">
         <v>0</v>
@@ -4331,7 +4322,7 @@
         <v>12</v>
       </c>
       <c r="C31" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D31">
         <v>0</v>
@@ -4348,7 +4339,7 @@
         <v>12</v>
       </c>
       <c r="C32" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
       <c r="D32">
         <v>0</v>
@@ -4365,7 +4356,7 @@
         <v>12</v>
       </c>
       <c r="C33" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D33">
         <v>0</v>
@@ -4382,7 +4373,7 @@
         <v>12</v>
       </c>
       <c r="C34" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D34">
         <v>0</v>
@@ -4399,7 +4390,7 @@
         <v>12</v>
       </c>
       <c r="C35" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="D35">
         <v>0</v>
@@ -4416,7 +4407,7 @@
         <v>12</v>
       </c>
       <c r="C36" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D36">
         <v>0</v>
@@ -4433,7 +4424,7 @@
         <v>12</v>
       </c>
       <c r="C37" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D37">
         <v>0</v>
@@ -4450,7 +4441,7 @@
         <v>12</v>
       </c>
       <c r="C38" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D38">
         <v>0</v>
@@ -4467,7 +4458,7 @@
         <v>12</v>
       </c>
       <c r="C39" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="D39">
         <v>0</v>
@@ -4484,7 +4475,7 @@
         <v>12</v>
       </c>
       <c r="C40" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D40">
         <v>0</v>
@@ -4501,7 +4492,7 @@
         <v>12</v>
       </c>
       <c r="C41" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D41">
         <v>0</v>
@@ -4518,7 +4509,7 @@
         <v>12</v>
       </c>
       <c r="C42" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="D42">
         <v>0</v>
@@ -4535,7 +4526,7 @@
         <v>12</v>
       </c>
       <c r="C43" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D43">
         <v>0</v>
@@ -4552,7 +4543,7 @@
         <v>12</v>
       </c>
       <c r="C44" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="D44">
         <v>0</v>
@@ -4569,7 +4560,7 @@
         <v>12</v>
       </c>
       <c r="C45" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D45">
         <v>0</v>
@@ -4586,7 +4577,7 @@
         <v>12</v>
       </c>
       <c r="C46" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D46">
         <v>0</v>
@@ -4603,7 +4594,7 @@
         <v>12</v>
       </c>
       <c r="C47" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D47">
         <v>0</v>
@@ -4620,7 +4611,7 @@
         <v>12</v>
       </c>
       <c r="C48" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
       <c r="D48">
         <v>0</v>
@@ -4637,7 +4628,7 @@
         <v>12</v>
       </c>
       <c r="C49" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D49">
         <v>0</v>
@@ -4654,7 +4645,7 @@
         <v>12</v>
       </c>
       <c r="C50" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
       <c r="D50">
         <v>0</v>
@@ -4671,7 +4662,7 @@
         <v>12</v>
       </c>
       <c r="C51" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D51">
         <v>0</v>
@@ -4688,7 +4679,7 @@
         <v>12</v>
       </c>
       <c r="C52" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
       <c r="D52">
         <v>0</v>
@@ -4705,7 +4696,7 @@
         <v>12</v>
       </c>
       <c r="C53" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D53">
         <v>0</v>
@@ -4722,7 +4713,7 @@
         <v>12</v>
       </c>
       <c r="C54" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
       <c r="D54">
         <v>0</v>
@@ -4739,7 +4730,7 @@
         <v>12</v>
       </c>
       <c r="C55" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D55">
         <v>0</v>
@@ -4756,7 +4747,7 @@
         <v>12</v>
       </c>
       <c r="C56" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D56">
         <v>0</v>
@@ -4773,7 +4764,7 @@
         <v>12</v>
       </c>
       <c r="C57" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
       <c r="D57">
         <v>0</v>
@@ -4790,7 +4781,7 @@
         <v>12</v>
       </c>
       <c r="C58" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D58">
         <v>0</v>
@@ -4807,7 +4798,7 @@
         <v>12</v>
       </c>
       <c r="C59" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="D59">
         <v>0</v>
@@ -4824,7 +4815,7 @@
         <v>12</v>
       </c>
       <c r="C60" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D60">
         <v>0</v>
@@ -4841,7 +4832,7 @@
         <v>12</v>
       </c>
       <c r="C61" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="D61">
         <v>0</v>
@@ -4858,7 +4849,7 @@
         <v>12</v>
       </c>
       <c r="C62" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D62">
         <v>0</v>
@@ -4875,7 +4866,7 @@
         <v>12</v>
       </c>
       <c r="C63" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="D63">
         <v>0</v>
@@ -4892,7 +4883,7 @@
         <v>12</v>
       </c>
       <c r="C64" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D64">
         <v>0</v>
@@ -4909,7 +4900,7 @@
         <v>12</v>
       </c>
       <c r="C65" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="D65">
         <v>0</v>
@@ -4926,7 +4917,7 @@
         <v>12</v>
       </c>
       <c r="C66" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D66">
         <v>0</v>
@@ -4943,7 +4934,7 @@
         <v>12</v>
       </c>
       <c r="C67" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="D67">
         <v>0</v>
@@ -4960,7 +4951,7 @@
         <v>12</v>
       </c>
       <c r="C68" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -4977,7 +4968,7 @@
         <v>12</v>
       </c>
       <c r="C69" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
       <c r="D69">
         <v>0</v>
@@ -4994,7 +4985,7 @@
         <v>12</v>
       </c>
       <c r="C70" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -5011,7 +5002,7 @@
         <v>12</v>
       </c>
       <c r="C71" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="D71">
         <v>0</v>
@@ -5028,7 +5019,7 @@
         <v>12</v>
       </c>
       <c r="C72" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D72">
         <v>0</v>
@@ -5045,7 +5036,7 @@
         <v>12</v>
       </c>
       <c r="C73" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D73">
         <v>0</v>
@@ -5062,7 +5053,7 @@
         <v>12</v>
       </c>
       <c r="C74" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D74">
         <v>0</v>
@@ -5079,7 +5070,7 @@
         <v>12</v>
       </c>
       <c r="C75" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D75">
         <v>0</v>
@@ -5096,7 +5087,7 @@
         <v>12</v>
       </c>
       <c r="C76" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D76">
         <v>0</v>
@@ -5113,7 +5104,7 @@
         <v>12</v>
       </c>
       <c r="C77" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D77">
         <v>0</v>
@@ -5130,7 +5121,7 @@
         <v>12</v>
       </c>
       <c r="C78" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D78">
         <v>0</v>
@@ -5147,7 +5138,7 @@
         <v>12</v>
       </c>
       <c r="C79" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D79">
         <v>0</v>
@@ -5164,7 +5155,7 @@
         <v>12</v>
       </c>
       <c r="C80" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -5181,7 +5172,7 @@
         <v>12</v>
       </c>
       <c r="C81" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D81">
         <v>0</v>
@@ -5198,7 +5189,7 @@
         <v>12</v>
       </c>
       <c r="C82" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="D82">
         <v>0</v>
@@ -5215,7 +5206,7 @@
         <v>12</v>
       </c>
       <c r="C83" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D83">
         <v>0</v>
@@ -5232,7 +5223,7 @@
         <v>12</v>
       </c>
       <c r="C84" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D84">
         <v>0</v>
@@ -5249,7 +5240,7 @@
         <v>12</v>
       </c>
       <c r="C85" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="D85">
         <v>0</v>
@@ -5266,7 +5257,7 @@
         <v>12</v>
       </c>
       <c r="C86" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D86">
         <v>0</v>
@@ -5283,7 +5274,7 @@
         <v>12</v>
       </c>
       <c r="C87" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D87">
         <v>0</v>
@@ -5300,7 +5291,7 @@
         <v>12</v>
       </c>
       <c r="C88" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="D88">
         <v>0</v>
@@ -5317,7 +5308,7 @@
         <v>12</v>
       </c>
       <c r="C89" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D89">
         <v>0</v>
@@ -5334,7 +5325,7 @@
         <v>12</v>
       </c>
       <c r="C90" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D90">
         <v>0</v>
@@ -5351,7 +5342,7 @@
         <v>12</v>
       </c>
       <c r="C91" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D91">
         <v>0</v>
@@ -5368,7 +5359,7 @@
         <v>12</v>
       </c>
       <c r="C92" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D92">
         <v>0</v>
@@ -5385,7 +5376,7 @@
         <v>12</v>
       </c>
       <c r="C93" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D93">
         <v>0</v>
@@ -5402,7 +5393,7 @@
         <v>12</v>
       </c>
       <c r="C94" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D94">
         <v>0</v>
@@ -5419,7 +5410,7 @@
         <v>12</v>
       </c>
       <c r="C95" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D95">
         <v>0</v>
@@ -5436,7 +5427,7 @@
         <v>12</v>
       </c>
       <c r="C96" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D96">
         <v>0</v>
@@ -5453,7 +5444,7 @@
         <v>12</v>
       </c>
       <c r="C97" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -5470,7 +5461,7 @@
         <v>12</v>
       </c>
       <c r="C98" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D98">
         <v>0</v>
@@ -5487,7 +5478,7 @@
         <v>12</v>
       </c>
       <c r="C99" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D99">
         <v>0</v>
@@ -5504,7 +5495,7 @@
         <v>12</v>
       </c>
       <c r="C100" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D100">
         <v>0</v>
@@ -5521,7 +5512,7 @@
         <v>12</v>
       </c>
       <c r="C101" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D101">
         <v>0</v>
@@ -5538,7 +5529,7 @@
         <v>12</v>
       </c>
       <c r="C102" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D102">
         <v>0</v>
@@ -5555,7 +5546,7 @@
         <v>12</v>
       </c>
       <c r="C103" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D103">
         <v>0</v>
@@ -5572,7 +5563,7 @@
         <v>12</v>
       </c>
       <c r="C104" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D104">
         <v>0</v>
@@ -5589,7 +5580,7 @@
         <v>12</v>
       </c>
       <c r="C105" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="D105">
         <v>0</v>
@@ -5606,7 +5597,7 @@
         <v>12</v>
       </c>
       <c r="C106" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D106">
         <v>0</v>
@@ -5623,7 +5614,7 @@
         <v>12</v>
       </c>
       <c r="C107" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D107">
         <v>0</v>
@@ -5640,7 +5631,7 @@
         <v>12</v>
       </c>
       <c r="C108" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="D108">
         <v>0</v>
@@ -5657,7 +5648,7 @@
         <v>12</v>
       </c>
       <c r="C109" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D109">
         <v>0</v>
@@ -5674,7 +5665,7 @@
         <v>12</v>
       </c>
       <c r="C110" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D110">
         <v>0</v>
@@ -5691,7 +5682,7 @@
         <v>12</v>
       </c>
       <c r="C111" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D111">
         <v>0</v>
@@ -5708,7 +5699,7 @@
         <v>12</v>
       </c>
       <c r="C112" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D112">
         <v>0</v>
@@ -5725,7 +5716,7 @@
         <v>12</v>
       </c>
       <c r="C113" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D113">
         <v>0</v>
@@ -5742,7 +5733,7 @@
         <v>12</v>
       </c>
       <c r="C114" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="D114">
         <v>0</v>
@@ -5759,7 +5750,7 @@
         <v>12</v>
       </c>
       <c r="C115" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D115">
         <v>0</v>
@@ -5776,7 +5767,7 @@
         <v>12</v>
       </c>
       <c r="C116" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D116">
         <v>0</v>
@@ -5793,7 +5784,7 @@
         <v>12</v>
       </c>
       <c r="C117" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="D117">
         <v>0</v>
@@ -5810,7 +5801,7 @@
         <v>12</v>
       </c>
       <c r="C118" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D118">
         <v>0</v>
@@ -5827,7 +5818,7 @@
         <v>12</v>
       </c>
       <c r="C119" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D119">
         <v>0</v>
@@ -5844,7 +5835,7 @@
         <v>12</v>
       </c>
       <c r="C120" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D120">
         <v>0</v>
@@ -5861,7 +5852,7 @@
         <v>12</v>
       </c>
       <c r="C121" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="D121">
         <v>0</v>
@@ -5878,7 +5869,7 @@
         <v>12</v>
       </c>
       <c r="C122" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D122">
         <v>0</v>
@@ -5895,7 +5886,7 @@
         <v>12</v>
       </c>
       <c r="C123" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="D123">
         <v>0</v>
@@ -5912,7 +5903,7 @@
         <v>12</v>
       </c>
       <c r="C124" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D124">
         <v>0</v>
@@ -5929,7 +5920,7 @@
         <v>12</v>
       </c>
       <c r="C125" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="D125">
         <v>0</v>
@@ -5946,7 +5937,7 @@
         <v>12</v>
       </c>
       <c r="C126" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D126">
         <v>0</v>
@@ -5963,7 +5954,7 @@
         <v>12</v>
       </c>
       <c r="C127" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="D127">
         <v>0</v>
@@ -5973,40 +5964,6 @@
       </c>
       <c r="F127" t="s">
         <v>215</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
-        <v>12</v>
-      </c>
-      <c r="C128" t="s">
-        <v>344</v>
-      </c>
-      <c r="D128">
-        <v>0</v>
-      </c>
-      <c r="E128">
-        <v>0</v>
-      </c>
-      <c r="F128" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
-        <v>12</v>
-      </c>
-      <c r="C129" t="s">
-        <v>344</v>
-      </c>
-      <c r="D129">
-        <v>0</v>
-      </c>
-      <c r="E129">
-        <v>1</v>
-      </c>
-      <c r="F129" t="s">
-        <v>262</v>
       </c>
     </row>
   </sheetData>

</xml_diff>